<commit_message>
Update Rizka - Data Binding Lihat Status Pengajuan Data Ketinggalan
</commit_message>
<xml_diff>
--- a/LihatStatusPengajuan.xlsx
+++ b/LihatStatusPengajuan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD4590F-D3FC-443D-B6DF-E35984156722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE824B1-5023-41B2-9F90-D0D3AF154709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="0" windowWidth="17895" windowHeight="11070" xr2:uid="{47EAEB65-58AE-4DFF-B37B-DDCDF32E8CCA}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="13440" windowHeight="11070" xr2:uid="{47EAEB65-58AE-4DFF-B37B-DDCDF32E8CCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>namaMobil</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Agya</t>
   </si>
   <si>
-    <t>Calya</t>
-  </si>
-  <si>
-    <t>Daihatsu New Ayla</t>
-  </si>
-  <si>
     <t>Brio</t>
   </si>
   <si>
@@ -60,6 +54,9 @@
   </si>
   <si>
     <t>searchByScroll</t>
+  </si>
+  <si>
+    <t>Kijang Innova</t>
   </si>
 </sst>
 </file>
@@ -494,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582AE73E-4E7C-4C63-9062-C5130DE9C190}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,31 +516,23 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>